<commit_message>
Updating GDP and GVA posts for 2024Q2 data
</commit_message>
<xml_diff>
--- a/posts/GDP_India/india-gdp.xlsx
+++ b/posts/GDP_India/india-gdp.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://liunet-my.sharepoint.com/personal/udayan_roy_liu_edu/Documents/Documents/data-miscellaneous/GDP-India/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="602" documentId="13_ncr:1_{EBE39D18-E49E-4C79-BE14-6F3DA64123A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{540406CC-9078-4CFA-B7EC-44A74897F46E}"/>
+  <xr:revisionPtr revIDLastSave="638" documentId="13_ncr:1_{EBE39D18-E49E-4C79-BE14-6F3DA64123A5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{6715785A-43F3-483D-A272-1904B8771AB0}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="11500" firstSheet="3" activeTab="5" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -257,7 +257,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="626" uniqueCount="253">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="628" uniqueCount="253">
   <si>
     <t>GDP (2011-12 Rupees, tens of millions)</t>
   </si>
@@ -1203,7 +1203,7 @@
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0"/>
     <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="34">
+  <cellXfs count="35">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
@@ -1264,6 +1264,7 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="1" xfId="0" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="2" applyNumberFormat="1" applyFont="1"/>
   </cellXfs>
   <cellStyles count="3">
     <cellStyle name="Comma" xfId="2" builtinId="3"/>
@@ -15527,11 +15528,11 @@
 
 <file path=xl/worksheets/sheet6.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0400-000000000000}">
-  <dimension ref="A1:AE56"/>
+  <dimension ref="A1:AE55"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="I1" workbookViewId="0">
-      <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="O12" sqref="O12"/>
+    <sheetView tabSelected="1" topLeftCell="P1" workbookViewId="0">
+      <pane ySplit="1" topLeftCell="A38" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="AA59" sqref="AA59"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -15739,15 +15740,15 @@
         <v>1</v>
       </c>
       <c r="AB2" s="31">
-        <f>P2-Y2</f>
+        <f t="shared" ref="AB2:AB33" si="3">P2-Y2</f>
         <v>0</v>
       </c>
       <c r="AC2" s="31">
-        <f>N2-(C2+F2+J2)</f>
+        <f t="shared" ref="AC2:AC47" si="4">N2-(C2+F2+J2)</f>
         <v>0</v>
       </c>
       <c r="AD2" s="13">
-        <f>P2-N2-O2</f>
+        <f t="shared" ref="AD2:AD33" si="5">P2-N2-O2</f>
         <v>133730.3899999999</v>
       </c>
     </row>
@@ -15834,15 +15835,15 @@
         <v>2</v>
       </c>
       <c r="AB3" s="31">
-        <f>P3-Y3</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC3" s="31">
-        <f>N3-(C3+F3+J3)</f>
+        <f t="shared" si="4"/>
         <v>2.0000000018626451E-2</v>
       </c>
       <c r="AD3" s="31">
-        <f>P3-N3-O3</f>
+        <f t="shared" si="5"/>
         <v>129663.02000000002</v>
       </c>
     </row>
@@ -15929,15 +15930,15 @@
         <v>3</v>
       </c>
       <c r="AB4" s="31">
-        <f>P4-Y4</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC4" s="31">
-        <f>N4-(C4+F4+J4)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD4" s="31">
-        <f>P4-N4-O4</f>
+        <f t="shared" si="5"/>
         <v>151239.69999999995</v>
       </c>
     </row>
@@ -16024,15 +16025,15 @@
         <v>4</v>
       </c>
       <c r="AB5" s="31">
-        <f>P5-Y5</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC5" s="31">
-        <f>N5-(C5+F5+J5)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD5" s="31">
-        <f>P5-N5-O5</f>
+        <f t="shared" si="5"/>
         <v>214749.83999999985</v>
       </c>
     </row>
@@ -16044,7 +16045,7 @@
         <v>1</v>
       </c>
       <c r="C6" s="13">
-        <f t="shared" ref="C6:C54" si="3">D6+E6</f>
+        <f t="shared" ref="C6:C54" si="6">D6+E6</f>
         <v>411979.36</v>
       </c>
       <c r="D6" s="13">
@@ -16119,15 +16120,15 @@
         <v>1</v>
       </c>
       <c r="AB6" s="31">
-        <f>P6-Y6</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC6" s="31">
-        <f>N6-(C6+F6+J6)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD6" s="31">
-        <f>P6-N6-O6</f>
+        <f t="shared" si="5"/>
         <v>130634.27000000002</v>
       </c>
     </row>
@@ -16139,7 +16140,7 @@
         <v>2</v>
       </c>
       <c r="C7" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>329980.7</v>
       </c>
       <c r="D7" s="13">
@@ -16214,15 +16215,15 @@
         <v>2</v>
       </c>
       <c r="AB7" s="31">
-        <f>P7-Y7</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC7" s="31">
-        <f>N7-(C7+F7+J7)</f>
+        <f t="shared" si="4"/>
         <v>1.0000000009313226E-2</v>
       </c>
       <c r="AD7" s="31">
-        <f>P7-N7-O7</f>
+        <f t="shared" si="5"/>
         <v>148037.14999999991</v>
       </c>
     </row>
@@ -16234,7 +16235,7 @@
         <v>3</v>
       </c>
       <c r="C8" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>570907.46</v>
       </c>
       <c r="D8" s="13">
@@ -16309,15 +16310,15 @@
         <v>3</v>
       </c>
       <c r="AB8" s="31">
-        <f>P8-Y8</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC8" s="31">
-        <f>N8-(C8+F8+J8)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD8" s="31">
-        <f>P8-N8-O8</f>
+        <f t="shared" si="5"/>
         <v>167239.00999999978</v>
       </c>
     </row>
@@ -16329,7 +16330,7 @@
         <v>4</v>
       </c>
       <c r="C9" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>474029.63</v>
       </c>
       <c r="D9" s="13">
@@ -16404,15 +16405,15 @@
         <v>4</v>
       </c>
       <c r="AB9" s="31">
-        <f>P9-Y9</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC9" s="31">
-        <f>N9-(C9+F9+J9)</f>
+        <f t="shared" si="4"/>
         <v>-9.9999997764825821E-3</v>
       </c>
       <c r="AD9" s="31">
-        <f>P9-N9-O9</f>
+        <f t="shared" si="5"/>
         <v>220830.87999999989</v>
       </c>
     </row>
@@ -16424,7 +16425,7 @@
         <v>1</v>
       </c>
       <c r="C10" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>422583.46</v>
       </c>
       <c r="D10" s="13">
@@ -16499,15 +16500,15 @@
         <v>1</v>
       </c>
       <c r="AB10" s="31">
-        <f>P10-Y10</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC10" s="31">
-        <f>N10-(C10+F10+J10)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD10" s="31">
-        <f>P10-N10-O10</f>
+        <f t="shared" si="5"/>
         <v>141166.78000000026</v>
       </c>
     </row>
@@ -16519,7 +16520,7 @@
         <v>2</v>
       </c>
       <c r="C11" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>345026.27999999997</v>
       </c>
       <c r="D11" s="13">
@@ -16594,15 +16595,15 @@
         <v>2</v>
       </c>
       <c r="AB11" s="31">
-        <f>P11-Y11</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC11" s="31">
-        <f>N11-(C11+F11+J11)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD11" s="31">
-        <f>P11-N11-O11</f>
+        <f t="shared" si="5"/>
         <v>163181.66000000015</v>
       </c>
     </row>
@@ -16614,7 +16615,7 @@
         <v>3</v>
       </c>
       <c r="C12" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>603779.52</v>
       </c>
       <c r="D12" s="13">
@@ -16689,15 +16690,15 @@
         <v>3</v>
       </c>
       <c r="AB12" s="31">
-        <f>P12-Y12</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC12" s="31">
-        <f>N12-(C12+F12+J12)</f>
+        <f t="shared" si="4"/>
         <v>2.0000000018626451E-2</v>
       </c>
       <c r="AD12" s="31">
-        <f>P12-N12-O12</f>
+        <f t="shared" si="5"/>
         <v>183056.38999999966</v>
       </c>
     </row>
@@ -16709,7 +16710,7 @@
         <v>4</v>
       </c>
       <c r="C13" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>500915.09</v>
       </c>
       <c r="D13" s="13">
@@ -16784,15 +16785,15 @@
         <v>4</v>
       </c>
       <c r="AB13" s="31">
-        <f>P13-Y13</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC13" s="31">
-        <f>N13-(C13+F13+J13)</f>
+        <f t="shared" si="4"/>
         <v>-1.0000000242143869E-2</v>
       </c>
       <c r="AD13" s="31">
-        <f>P13-N13-O13</f>
+        <f t="shared" si="5"/>
         <v>250318.37000000011</v>
       </c>
     </row>
@@ -16804,7 +16805,7 @@
         <v>1</v>
       </c>
       <c r="C14" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>442188.55</v>
       </c>
       <c r="D14" s="13">
@@ -16879,15 +16880,15 @@
         <v>1</v>
       </c>
       <c r="AB14" s="31">
-        <f>P14-Y14</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC14" s="31">
-        <f>N14-(C14+F14+J14)</f>
+        <f t="shared" si="4"/>
         <v>2.0000000018626451E-2</v>
       </c>
       <c r="AD14" s="31">
-        <f>P14-N14-O14</f>
+        <f t="shared" si="5"/>
         <v>158596.73999999976</v>
       </c>
     </row>
@@ -16899,7 +16900,7 @@
         <v>2</v>
       </c>
       <c r="C15" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>357433.54000000004</v>
       </c>
       <c r="D15" s="13">
@@ -16974,15 +16975,15 @@
         <v>2</v>
       </c>
       <c r="AB15" s="31">
-        <f>P15-Y15</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC15" s="31">
-        <f>N15-(C15+F15+J15)</f>
+        <f t="shared" si="4"/>
         <v>9.9999997764825821E-3</v>
       </c>
       <c r="AD15" s="31">
-        <f>P15-N15-O15</f>
+        <f t="shared" si="5"/>
         <v>182885.76000000024</v>
       </c>
     </row>
@@ -16994,7 +16995,7 @@
         <v>3</v>
       </c>
       <c r="C16" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>591556.76</v>
       </c>
       <c r="D16" s="13">
@@ -17069,15 +17070,15 @@
         <v>3</v>
       </c>
       <c r="AB16" s="31">
-        <f>P16-Y16</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC16" s="31">
-        <f>N16-(C16+F16+J16)</f>
+        <f t="shared" si="4"/>
         <v>1.0000000242143869E-2</v>
       </c>
       <c r="AD16" s="31">
-        <f>P16-N16-O16</f>
+        <f t="shared" si="5"/>
         <v>188936.89000000013</v>
       </c>
     </row>
@@ -17089,7 +17090,7 @@
         <v>4</v>
       </c>
       <c r="C17" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>503220.85</v>
       </c>
       <c r="D17" s="13">
@@ -17164,15 +17165,15 @@
         <v>4</v>
       </c>
       <c r="AB17" s="31">
-        <f>P17-Y17</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC17" s="31">
-        <f>N17-(C17+F17+J17)</f>
+        <f t="shared" si="4"/>
         <v>2.0000000018626451E-2</v>
       </c>
       <c r="AD17" s="31">
-        <f>P17-N17-O17</f>
+        <f t="shared" si="5"/>
         <v>285121.45000000019</v>
       </c>
     </row>
@@ -17184,7 +17185,7 @@
         <v>1</v>
       </c>
       <c r="C18" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>458457.33</v>
       </c>
       <c r="D18" s="13">
@@ -17259,15 +17260,15 @@
         <v>1</v>
       </c>
       <c r="AB18" s="31">
-        <f>P18-Y18</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC18" s="31">
-        <f>N18-(C18+F18+J18)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD18" s="31">
-        <f>P18-N18-O18</f>
+        <f t="shared" si="5"/>
         <v>168087.37000000011</v>
       </c>
     </row>
@@ -17279,7 +17280,7 @@
         <v>2</v>
       </c>
       <c r="C19" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>371275.52000000002</v>
       </c>
       <c r="D19" s="13">
@@ -17354,15 +17355,15 @@
         <v>2</v>
       </c>
       <c r="AB19" s="31">
-        <f>P19-Y19</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC19" s="31">
-        <f>N19-(C19+F19+J19)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD19" s="31">
-        <f>P19-N19-O19</f>
+        <f t="shared" si="5"/>
         <v>189862.4700000002</v>
       </c>
     </row>
@@ -17374,7 +17375,7 @@
         <v>3</v>
       </c>
       <c r="C20" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>587427.96</v>
       </c>
       <c r="D20" s="13">
@@ -17449,15 +17450,15 @@
         <v>3</v>
       </c>
       <c r="AB20" s="31">
-        <f>P20-Y20</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC20" s="31">
-        <f>N20-(C20+F20+J20)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD20" s="31">
-        <f>P20-N20-O20</f>
+        <f t="shared" si="5"/>
         <v>199383.31000000006</v>
       </c>
     </row>
@@ -17469,7 +17470,7 @@
         <v>4</v>
       </c>
       <c r="C21" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>516958.92</v>
       </c>
       <c r="D21" s="13">
@@ -17544,15 +17545,15 @@
         <v>4</v>
       </c>
       <c r="AB21" s="31">
-        <f>P21-Y21</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC21" s="31">
-        <f>N21-(C21+F21+J21)</f>
+        <f t="shared" si="4"/>
         <v>-1.0000000242143869E-2</v>
       </c>
       <c r="AD21" s="31">
-        <f>P21-N21-O21</f>
+        <f t="shared" si="5"/>
         <v>320289.63000000035</v>
       </c>
     </row>
@@ -17564,7 +17565,7 @@
         <v>1</v>
       </c>
       <c r="C22" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>482991.46</v>
       </c>
       <c r="D22" s="13">
@@ -17639,15 +17640,15 @@
         <v>1</v>
       </c>
       <c r="AB22" s="31">
-        <f>P22-Y22</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC22" s="31">
-        <f>N22-(C22+F22+J22)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD22" s="31">
-        <f>P22-N22-O22</f>
+        <f t="shared" si="5"/>
         <v>166361.40999999968</v>
       </c>
     </row>
@@ -17659,7 +17660,7 @@
         <v>2</v>
       </c>
       <c r="C23" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>394209.86</v>
       </c>
       <c r="D23" s="13">
@@ -17734,15 +17735,15 @@
         <v>2</v>
       </c>
       <c r="AB23" s="31">
-        <f>P23-Y23</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC23" s="31">
-        <f>N23-(C23+F23+J23)</f>
+        <f t="shared" si="4"/>
         <v>1.0000000242143869E-2</v>
       </c>
       <c r="AD23" s="31">
-        <f>P23-N23-O23</f>
+        <f t="shared" si="5"/>
         <v>243762.10999999987</v>
       </c>
     </row>
@@ -17754,7 +17755,7 @@
         <v>3</v>
       </c>
       <c r="C24" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>631950.26</v>
       </c>
       <c r="D24" s="13">
@@ -17829,15 +17830,15 @@
         <v>3</v>
       </c>
       <c r="AB24" s="31">
-        <f>P24-Y24</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC24" s="31">
-        <f>N24-(C24+F24+J24)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD24" s="31">
-        <f>P24-N24-O24</f>
+        <f t="shared" si="5"/>
         <v>244007.54999999981</v>
       </c>
     </row>
@@ -17849,7 +17850,7 @@
         <v>4</v>
       </c>
       <c r="C25" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>566099.98</v>
       </c>
       <c r="D25" s="13">
@@ -17924,15 +17925,15 @@
         <v>4</v>
       </c>
       <c r="AB25" s="31">
-        <f>P25-Y25</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC25" s="31">
-        <f>N25-(C25+F25+J25)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD25" s="31">
-        <f>P25-N25-O25</f>
+        <f t="shared" si="5"/>
         <v>325777.52</v>
       </c>
     </row>
@@ -17944,7 +17945,7 @@
         <v>1</v>
       </c>
       <c r="C26" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>497397.44</v>
       </c>
       <c r="D26" s="13">
@@ -18019,15 +18020,15 @@
         <v>1</v>
       </c>
       <c r="AB26" s="31">
-        <f>P26-Y26</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC26" s="31">
-        <f>N26-(C26+F26+J26)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD26" s="31">
-        <f>P26-N26-O26</f>
+        <f t="shared" si="5"/>
         <v>208228.82999999961</v>
       </c>
     </row>
@@ -18039,7 +18040,7 @@
         <v>2</v>
       </c>
       <c r="C27" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>418669.19</v>
       </c>
       <c r="D27" s="13">
@@ -18114,15 +18115,15 @@
         <v>2</v>
       </c>
       <c r="AB27" s="31">
-        <f>P27-Y27</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC27" s="31">
-        <f>N27-(C27+F27+J27)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD27" s="31">
-        <f>P27-N27-O27</f>
+        <f t="shared" si="5"/>
         <v>250525.44000000041</v>
       </c>
     </row>
@@ -18134,7 +18135,7 @@
         <v>3</v>
       </c>
       <c r="C28" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>660765.02999999991</v>
       </c>
       <c r="D28" s="13">
@@ -18209,15 +18210,15 @@
         <v>3</v>
       </c>
       <c r="AB28" s="31">
-        <f>P28-Y28</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC28" s="31">
-        <f>N28-(C28+F28+J28)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD28" s="31">
-        <f>P28-N28-O28</f>
+        <f t="shared" si="5"/>
         <v>252196.64000000013</v>
       </c>
     </row>
@@ -18229,7 +18230,7 @@
         <v>4</v>
       </c>
       <c r="C29" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>592803.28</v>
       </c>
       <c r="D29" s="13">
@@ -18304,15 +18305,15 @@
         <v>4</v>
       </c>
       <c r="AB29" s="31">
-        <f>P29-Y29</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC29" s="31">
-        <f>N29-(C29+F29+J29)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD29" s="31">
-        <f>P29-N29-O29</f>
+        <f t="shared" si="5"/>
         <v>399460.35999999987</v>
       </c>
     </row>
@@ -18324,7 +18325,7 @@
         <v>1</v>
       </c>
       <c r="C30" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>516246.14</v>
       </c>
       <c r="D30" s="13">
@@ -18399,15 +18400,15 @@
         <v>1</v>
       </c>
       <c r="AB30" s="31">
-        <f>P30-Y30</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC30" s="31">
-        <f>N30-(C30+F30+J30)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD30" s="31">
-        <f>P30-N30-O30</f>
+        <f t="shared" si="5"/>
         <v>235157.8200000003</v>
       </c>
     </row>
@@ -18419,7 +18420,7 @@
         <v>2</v>
       </c>
       <c r="C31" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>432086.64</v>
       </c>
       <c r="D31" s="13">
@@ -18494,15 +18495,15 @@
         <v>2</v>
       </c>
       <c r="AB31" s="31">
-        <f>P31-Y31</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC31" s="31">
-        <f>N31-(C31+F31+J31)</f>
+        <f t="shared" si="4"/>
         <v>-9.9999997764825821E-3</v>
       </c>
       <c r="AD31" s="31">
-        <f>P31-N31-O31</f>
+        <f t="shared" si="5"/>
         <v>276091.19999999972</v>
       </c>
     </row>
@@ -18514,7 +18515,7 @@
         <v>3</v>
       </c>
       <c r="C32" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>668515.21</v>
       </c>
       <c r="D32" s="13">
@@ -18589,15 +18590,15 @@
         <v>3</v>
       </c>
       <c r="AB32" s="31">
-        <f>P32-Y32</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC32" s="31">
-        <f>N32-(C32+F32+J32)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD32" s="31">
-        <f>P32-N32-O32</f>
+        <f t="shared" si="5"/>
         <v>296663.66000000015</v>
       </c>
     </row>
@@ -18609,7 +18610,7 @@
         <v>4</v>
       </c>
       <c r="C33" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>588566.93999999994</v>
       </c>
       <c r="D33" s="13">
@@ -18684,15 +18685,15 @@
         <v>4</v>
       </c>
       <c r="AB33" s="31">
-        <f>P33-Y33</f>
+        <f t="shared" si="3"/>
         <v>0</v>
       </c>
       <c r="AC33" s="31">
-        <f>N33-(C33+F33+J33)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD33" s="31">
-        <f>P33-N33-O33</f>
+        <f t="shared" si="5"/>
         <v>451203.49000000022</v>
       </c>
     </row>
@@ -18704,7 +18705,7 @@
         <v>1</v>
       </c>
       <c r="C34" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>531399.76</v>
       </c>
       <c r="D34" s="13">
@@ -18714,7 +18715,7 @@
         <v>82696.429999999993</v>
       </c>
       <c r="F34" s="13">
-        <f t="shared" ref="F34:F54" si="4">SUM(G34:I34)</f>
+        <f t="shared" ref="F34:F54" si="7">SUM(G34:I34)</f>
         <v>904947.13</v>
       </c>
       <c r="G34" s="13">
@@ -18779,15 +18780,15 @@
         <v>1</v>
       </c>
       <c r="AB34" s="31">
-        <f>P34-Y34</f>
+        <f t="shared" ref="AB34:AB54" si="8">P34-Y34</f>
         <v>0</v>
       </c>
       <c r="AC34" s="31">
-        <f>N34-(C34+F34+J34)</f>
+        <f t="shared" si="4"/>
         <v>-1.0000000242143869E-2</v>
       </c>
       <c r="AD34" s="31">
-        <f>P34-N34-O34</f>
+        <f t="shared" ref="AD34:AD54" si="9">P34-N34-O34</f>
         <v>261086.70999999996</v>
       </c>
     </row>
@@ -18799,7 +18800,7 @@
         <v>2</v>
       </c>
       <c r="C35" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>446471.92000000004</v>
       </c>
       <c r="D35" s="13">
@@ -18809,7 +18810,7 @@
         <v>65070.66</v>
       </c>
       <c r="F35" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>881110.07</v>
       </c>
       <c r="G35" s="13">
@@ -18874,15 +18875,15 @@
         <v>2</v>
       </c>
       <c r="AB35" s="31">
-        <f>P35-Y35</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC35" s="31">
-        <f>N35-(C35+F35+J35)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD35" s="31">
-        <f>P35-N35-O35</f>
+        <f t="shared" si="9"/>
         <v>289713.48</v>
       </c>
     </row>
@@ -18894,7 +18895,7 @@
         <v>3</v>
       </c>
       <c r="C36" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>698338.2</v>
       </c>
       <c r="D36" s="13">
@@ -18904,7 +18905,7 @@
         <v>77460.100000000006</v>
       </c>
       <c r="F36" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>872947.08000000007</v>
       </c>
       <c r="G36" s="13">
@@ -18969,15 +18970,15 @@
         <v>3</v>
       </c>
       <c r="AB36" s="31">
-        <f>P36-Y36</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC36" s="31">
-        <f>N36-(C36+F36+J36)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD36" s="31">
-        <f>P36-N36-O36</f>
+        <f t="shared" si="9"/>
         <v>302203.8200000003</v>
       </c>
     </row>
@@ -18989,7 +18990,7 @@
         <v>4</v>
       </c>
       <c r="C37" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>627859.40999999992</v>
       </c>
       <c r="D37" s="13">
@@ -18999,7 +19000,7 @@
         <v>96539.19</v>
       </c>
       <c r="F37" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>941644.3</v>
       </c>
       <c r="G37" s="13">
@@ -19064,15 +19065,15 @@
         <v>4</v>
       </c>
       <c r="AB37" s="31">
-        <f>P37-Y37</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC37" s="31">
-        <f>N37-(C37+F37+J37)</f>
+        <f t="shared" si="4"/>
         <v>-1.0000000242143869E-2</v>
       </c>
       <c r="AD37" s="31">
-        <f>P37-N37-O37</f>
+        <f t="shared" si="9"/>
         <v>443478.06000000006</v>
       </c>
     </row>
@@ -19084,7 +19085,7 @@
         <v>1</v>
       </c>
       <c r="C38" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>530005.9</v>
       </c>
       <c r="D38" s="13">
@@ -19094,7 +19095,7 @@
         <v>67999.62</v>
       </c>
       <c r="F38" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>586786.70000000007</v>
       </c>
       <c r="G38" s="13">
@@ -19159,15 +19160,15 @@
         <v>1</v>
       </c>
       <c r="AB38" s="31">
-        <f>P38-Y38</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC38" s="31">
-        <f>N38-(C38+F38+J38)</f>
+        <f t="shared" si="4"/>
         <v>9.9999997764825821E-3</v>
       </c>
       <c r="AD38" s="31">
-        <f>P38-N38-O38</f>
+        <f t="shared" si="9"/>
         <v>119796.79000000004</v>
       </c>
     </row>
@@ -19179,7 +19180,7 @@
         <v>2</v>
       </c>
       <c r="C39" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>453340.4</v>
       </c>
       <c r="D39" s="13">
@@ -19189,7 +19190,7 @@
         <v>59916.25</v>
       </c>
       <c r="F39" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>891821.99000000011</v>
       </c>
       <c r="G39" s="13">
@@ -19254,15 +19255,15 @@
         <v>2</v>
       </c>
       <c r="AB39" s="31">
-        <f>P39-Y39</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC39" s="31">
-        <f>N39-(C39+F39+J39)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD39" s="31">
-        <f>P39-N39-O39</f>
+        <f t="shared" si="9"/>
         <v>246010.04999999981</v>
       </c>
     </row>
@@ -19274,7 +19275,7 @@
         <v>3</v>
       </c>
       <c r="C40" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>719623.93</v>
       </c>
       <c r="D40" s="13">
@@ -19284,7 +19285,7 @@
         <v>73346.39</v>
       </c>
       <c r="F40" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>936828.87</v>
       </c>
       <c r="G40" s="13">
@@ -19349,15 +19350,15 @@
         <v>3</v>
       </c>
       <c r="AB40" s="31">
-        <f>P40-Y40</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC40" s="31">
-        <f>N40-(C40+F40+J40)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD40" s="31">
-        <f>P40-N40-O40</f>
+        <f t="shared" si="9"/>
         <v>259909.15000000037</v>
       </c>
     </row>
@@ -19369,7 +19370,7 @@
         <v>4</v>
       </c>
       <c r="C41" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>639085.95000000007</v>
       </c>
       <c r="D41" s="13">
@@ -19379,7 +19380,7 @@
         <v>92762.03</v>
       </c>
       <c r="F41" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1084909.06</v>
       </c>
       <c r="G41" s="13">
@@ -19444,15 +19445,15 @@
         <v>4</v>
       </c>
       <c r="AB41" s="31">
-        <f>P41-Y41</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC41" s="31">
-        <f>N41-(C41+F41+J41)</f>
+        <f t="shared" si="4"/>
         <v>9.9999997764825821E-3</v>
       </c>
       <c r="AD41" s="31">
-        <f>P41-N41-O41</f>
+        <f t="shared" si="9"/>
         <v>347683.79999999981</v>
       </c>
     </row>
@@ -19464,7 +19465,7 @@
         <v>1</v>
       </c>
       <c r="C42" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>552500.73</v>
       </c>
       <c r="D42" s="13">
@@ -19474,7 +19475,7 @@
         <v>80242.81</v>
       </c>
       <c r="F42" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>879711.74</v>
       </c>
       <c r="G42" s="13">
@@ -19487,7 +19488,7 @@
         <v>225166.19</v>
       </c>
       <c r="J42" s="13">
-        <f t="shared" ref="J42:J52" si="5">SUM(K42:M42)</f>
+        <f t="shared" ref="J42:J52" si="10">SUM(K42:M42)</f>
         <v>1620451.6900000002</v>
       </c>
       <c r="K42" s="13">
@@ -19542,15 +19543,15 @@
         <v>1</v>
       </c>
       <c r="AB42" s="31">
-        <f>P42-Y42</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC42" s="13">
-        <f>N42-(C42+F42+J42)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD42" s="31">
-        <f>P42-N42-O42</f>
+        <f t="shared" si="9"/>
         <v>5588.1682359804399</v>
       </c>
     </row>
@@ -19562,7 +19563,7 @@
         <v>2</v>
       </c>
       <c r="C43" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>474496.35</v>
       </c>
       <c r="D43" s="13">
@@ -19572,7 +19573,7 @@
         <v>68626.06</v>
       </c>
       <c r="F43" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>949347.72</v>
       </c>
       <c r="G43" s="13">
@@ -19585,7 +19586,7 @@
         <v>243071.3</v>
       </c>
       <c r="J43" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1895404.18</v>
       </c>
       <c r="K43" s="13">
@@ -19640,15 +19641,15 @@
         <v>2</v>
       </c>
       <c r="AB43" s="31">
-        <f>P43-Y43</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC43" s="31">
-        <f>N43-(C43+F43+J43)</f>
+        <f t="shared" si="4"/>
         <v>9.9999997764825821E-3</v>
       </c>
       <c r="AD43" s="31">
-        <f>P43-N43-O43</f>
+        <f t="shared" si="9"/>
         <v>-5460.5229183249176</v>
       </c>
     </row>
@@ -19660,7 +19661,7 @@
         <v>3</v>
       </c>
       <c r="C44" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>742783.89999999991</v>
       </c>
       <c r="D44" s="13">
@@ -19670,7 +19671,7 @@
         <v>80095.429999999993</v>
       </c>
       <c r="F44" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>933564.98</v>
       </c>
       <c r="G44" s="13">
@@ -19683,7 +19684,7 @@
         <v>267074.26</v>
       </c>
       <c r="J44" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1848436.9699999997</v>
       </c>
       <c r="K44" s="13">
@@ -19738,15 +19739,15 @@
         <v>3</v>
       </c>
       <c r="AB44" s="31">
-        <f>P44-Y44</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC44" s="31">
-        <f>N44-(C44+F44+J44)</f>
+        <f t="shared" si="4"/>
         <v>0</v>
       </c>
       <c r="AD44" s="31">
-        <f>P44-N44-O44</f>
+        <f t="shared" si="9"/>
         <v>-3884.5467146392912</v>
       </c>
     </row>
@@ -19758,7 +19759,7 @@
         <v>4</v>
       </c>
       <c r="C45" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>667899.43000000005</v>
       </c>
       <c r="D45" s="13">
@@ -19768,7 +19769,7 @@
         <v>99019.54</v>
       </c>
       <c r="F45" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1093390.92</v>
       </c>
       <c r="G45" s="13">
@@ -19781,7 +19782,7 @@
         <v>338283.22</v>
       </c>
       <c r="J45" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1947485.4</v>
       </c>
       <c r="K45" s="13">
@@ -19836,214 +19837,215 @@
         <v>4</v>
       </c>
       <c r="AB45" s="31">
-        <f>P45-Y45</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC45" s="31">
-        <f>N45-(C45+F45+J45)</f>
+        <f t="shared" si="4"/>
         <v>-9.9999997764825821E-3</v>
       </c>
       <c r="AD45" s="31">
-        <f>P45-N45-O45</f>
+        <f t="shared" si="9"/>
         <v>-11207.842640354764</v>
       </c>
     </row>
-    <row r="46" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="46" spans="1:31" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A46" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="B46" s="13">
+      <c r="B46" s="22">
         <v>1</v>
       </c>
-      <c r="C46" s="13">
+      <c r="C46" s="22">
         <f>D46+E46</f>
         <v>582778.72476590949</v>
       </c>
-      <c r="D46" s="13">
+      <c r="D46" s="22">
         <v>502858.518800069</v>
       </c>
-      <c r="E46" s="13">
+      <c r="E46" s="22">
         <v>79920.205965840505</v>
       </c>
-      <c r="F46" s="13">
+      <c r="F46" s="22">
+        <f t="shared" si="7"/>
+        <v>1008980.4140133657</v>
+      </c>
+      <c r="G46" s="22">
+        <v>609517.77969751903</v>
+      </c>
+      <c r="H46" s="22">
+        <v>91144.538280434805</v>
+      </c>
+      <c r="I46" s="22">
+        <v>308318.09603541187</v>
+      </c>
+      <c r="J46" s="22">
+        <f t="shared" si="10"/>
+        <v>1929265.8061322137</v>
+      </c>
+      <c r="K46" s="22">
+        <v>588074.985123705</v>
+      </c>
+      <c r="L46" s="22">
+        <v>903193.87030003429</v>
+      </c>
+      <c r="M46" s="22">
+        <v>437996.95070847438</v>
+      </c>
+      <c r="N46" s="22">
+        <v>3521024.9449114874</v>
+      </c>
+      <c r="O46" s="22">
+        <v>258929.2627024604</v>
+      </c>
+      <c r="P46" s="22">
+        <v>3779954.2076139478</v>
+      </c>
+      <c r="Q46" s="22">
+        <v>2166247.8131295969</v>
+      </c>
+      <c r="R46" s="22">
+        <v>416509.07066349353</v>
+      </c>
+      <c r="S46" s="22">
+        <v>1303950.9268549108</v>
+      </c>
+      <c r="T46" s="22">
+        <v>44646.569579251096</v>
+      </c>
+      <c r="U46" s="22">
+        <v>35436.216201979827</v>
+      </c>
+      <c r="V46" s="22">
+        <v>935659.58990215987</v>
+      </c>
+      <c r="W46" s="22">
+        <v>959073.5694976236</v>
+      </c>
+      <c r="X46" s="22">
+        <v>-163422.40921982087</v>
+      </c>
+      <c r="Y46" s="22">
+        <v>3779954.2076139478</v>
+      </c>
+      <c r="Z46" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA46" s="22">
+        <v>1</v>
+      </c>
+      <c r="AB46" s="34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC46" s="34">
         <f t="shared" si="4"/>
-        <v>1008980.4140133657</v>
-      </c>
-      <c r="G46" s="13">
-        <v>609517.77969751903</v>
-      </c>
-      <c r="H46" s="13">
-        <v>91144.538280434805</v>
-      </c>
-      <c r="I46" s="13">
-        <v>308318.09603541187</v>
-      </c>
-      <c r="J46" s="13">
-        <f t="shared" si="5"/>
-        <v>1929265.8061322137</v>
-      </c>
-      <c r="K46" s="13">
-        <v>588074.985123705</v>
-      </c>
-      <c r="L46" s="13">
-        <v>903193.87030003429</v>
-      </c>
-      <c r="M46" s="13">
-        <v>437996.95070847438</v>
-      </c>
-      <c r="N46" s="13">
-        <v>3521024.9449114874</v>
-      </c>
-      <c r="O46" s="13">
-        <v>258929.2627024604</v>
-      </c>
-      <c r="P46" s="13">
-        <v>3779954.2076139478</v>
-      </c>
-      <c r="Q46" s="13">
-        <v>2166247.8131295969</v>
-      </c>
-      <c r="R46" s="13">
-        <v>416509.07066349353</v>
-      </c>
-      <c r="S46" s="13">
-        <v>1303950.9268549108</v>
-      </c>
-      <c r="T46" s="13">
-        <v>44646.569579251096</v>
-      </c>
-      <c r="U46" s="13">
-        <v>35436.216201979827</v>
-      </c>
-      <c r="V46" s="13">
-        <v>935659.58990215987</v>
-      </c>
-      <c r="W46" s="13">
-        <v>959073.5694976236</v>
-      </c>
-      <c r="X46" s="13">
-        <v>-163422.40921982087</v>
-      </c>
-      <c r="Y46" s="13">
-        <v>3779954.2076139478</v>
-      </c>
-      <c r="Z46" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA46" s="13">
-        <v>1</v>
-      </c>
-      <c r="AB46" s="31">
-        <f>P46-Y46</f>
         <v>0</v>
       </c>
-      <c r="AC46" s="31">
-        <f>N46-(C46+F46+J46)</f>
+      <c r="AD46" s="34">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AD46" s="31">
-        <f>P46-N46-O46</f>
-        <v>0</v>
-      </c>
-      <c r="AE46" s="13"/>
-    </row>
-    <row r="47" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AE46" s="22"/>
+    </row>
+    <row r="47" spans="1:31" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A47" s="30" t="s">
         <v>131</v>
       </c>
-      <c r="B47" s="13">
+      <c r="B47" s="22">
         <v>2</v>
       </c>
-      <c r="C47" s="13">
-        <f t="shared" si="3"/>
+      <c r="C47" s="22">
+        <f t="shared" si="6"/>
         <v>495503.03918673965</v>
       </c>
-      <c r="D47" s="13">
+      <c r="D47" s="22">
         <v>433438.82619629393</v>
       </c>
-      <c r="E47" s="13">
+      <c r="E47" s="22">
         <v>62064.212990445747</v>
       </c>
-      <c r="F47" s="13">
+      <c r="F47" s="22">
+        <f t="shared" si="7"/>
+        <v>971473.07053758157</v>
+      </c>
+      <c r="G47" s="22">
+        <v>601225.00399827119</v>
+      </c>
+      <c r="H47" s="22">
+        <v>88379.026389291161</v>
+      </c>
+      <c r="I47" s="22">
+        <v>281869.04015001917</v>
+      </c>
+      <c r="J47" s="22">
+        <f t="shared" si="10"/>
+        <v>2101128.930950419</v>
+      </c>
+      <c r="K47" s="22">
+        <v>677140.66039519641</v>
+      </c>
+      <c r="L47" s="22">
+        <v>952432.88935660443</v>
+      </c>
+      <c r="M47" s="22">
+        <v>471555.38119861821</v>
+      </c>
+      <c r="N47" s="22">
+        <v>3568105.04067474</v>
+      </c>
+      <c r="O47" s="22">
+        <v>304752.52294245921</v>
+      </c>
+      <c r="P47" s="22">
+        <v>3872857.5636171992</v>
+      </c>
+      <c r="Q47" s="22">
+        <v>2282920.0772977136</v>
+      </c>
+      <c r="R47" s="22">
+        <v>336707.36439945333</v>
+      </c>
+      <c r="S47" s="22">
+        <v>1285348.5529850633</v>
+      </c>
+      <c r="T47" s="22">
+        <v>44039.13202846246</v>
+      </c>
+      <c r="U47" s="22">
+        <v>109678.22609755064</v>
+      </c>
+      <c r="V47" s="22">
+        <v>948377.89428236673</v>
+      </c>
+      <c r="W47" s="22">
+        <v>1028800.0793153479</v>
+      </c>
+      <c r="X47" s="22">
+        <v>-105413.6041580626</v>
+      </c>
+      <c r="Y47" s="22">
+        <v>3872857.5636171992</v>
+      </c>
+      <c r="Z47" s="22" t="s">
+        <v>131</v>
+      </c>
+      <c r="AA47" s="22">
+        <v>2</v>
+      </c>
+      <c r="AB47" s="34">
+        <f t="shared" si="8"/>
+        <v>0</v>
+      </c>
+      <c r="AC47" s="34">
         <f t="shared" si="4"/>
-        <v>971473.07053758157</v>
-      </c>
-      <c r="G47" s="13">
-        <v>601225.00399827119</v>
-      </c>
-      <c r="H47" s="13">
-        <v>88379.026389291161</v>
-      </c>
-      <c r="I47" s="13">
-        <v>281869.04015001917</v>
-      </c>
-      <c r="J47" s="13">
-        <f t="shared" si="5"/>
-        <v>2101128.930950419</v>
-      </c>
-      <c r="K47" s="13">
-        <v>677140.66039519641</v>
-      </c>
-      <c r="L47" s="13">
-        <v>952432.88935660443</v>
-      </c>
-      <c r="M47" s="13">
-        <v>471555.38119861821</v>
-      </c>
-      <c r="N47" s="13">
-        <v>3568105.04067474</v>
-      </c>
-      <c r="O47" s="13">
-        <v>304752.52294245921</v>
-      </c>
-      <c r="P47" s="13">
-        <v>3872857.5636171992</v>
-      </c>
-      <c r="Q47" s="13">
-        <v>2282920.0772977136</v>
-      </c>
-      <c r="R47" s="13">
-        <v>336707.36439945333</v>
-      </c>
-      <c r="S47" s="13">
-        <v>1285348.5529850633</v>
-      </c>
-      <c r="T47" s="13">
-        <v>44039.13202846246</v>
-      </c>
-      <c r="U47" s="13">
-        <v>109678.22609755064</v>
-      </c>
-      <c r="V47" s="13">
-        <v>948377.89428236673</v>
-      </c>
-      <c r="W47" s="13">
-        <v>1028800.0793153479</v>
-      </c>
-      <c r="X47" s="13">
-        <v>-105413.6041580626</v>
-      </c>
-      <c r="Y47" s="13">
-        <v>3872857.5636171992</v>
-      </c>
-      <c r="Z47" s="13" t="s">
-        <v>131</v>
-      </c>
-      <c r="AA47" s="13">
-        <v>2</v>
-      </c>
-      <c r="AB47" s="31">
-        <f>P47-Y47</f>
         <v>0</v>
       </c>
-      <c r="AC47" s="31">
-        <f>N47-(C47+F47+J47)</f>
+      <c r="AD47" s="34">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AD47" s="31">
-        <f>P47-N47-O47</f>
-        <v>0</v>
-      </c>
+      <c r="AE47" s="22"/>
     </row>
     <row r="48" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A48" s="30" t="s">
@@ -20053,7 +20055,7 @@
         <v>3</v>
       </c>
       <c r="C48" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>785494.34019915422</v>
       </c>
       <c r="D48" s="13">
@@ -20063,7 +20065,7 @@
         <v>76876.763303309708</v>
       </c>
       <c r="F48" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>998134.35532813636</v>
       </c>
       <c r="G48" s="13">
@@ -20076,7 +20078,7 @@
         <v>329589.62111451046</v>
       </c>
       <c r="J48" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>1958004.7181515456</v>
       </c>
       <c r="K48" s="13">
@@ -20131,15 +20133,15 @@
         <v>3</v>
       </c>
       <c r="AB48" s="31">
-        <f>P48-Y48</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC48" s="31">
-        <f t="shared" ref="AC48:AC54" si="6">N48-(C48+F48+J48)</f>
+        <f t="shared" ref="AC48:AC54" si="11">N48-(C48+F48+J48)</f>
         <v>0</v>
       </c>
       <c r="AD48" s="31">
-        <f>P48-N48-O48</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -20161,7 +20163,7 @@
         <v>96395.089209460275</v>
       </c>
       <c r="F49" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1180304.7595683406</v>
       </c>
       <c r="G49" s="13">
@@ -20174,7 +20176,7 @@
         <v>386479.09900911065</v>
       </c>
       <c r="J49" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2070101.7898306134</v>
       </c>
       <c r="K49" s="13">
@@ -20229,214 +20231,215 @@
         <v>4</v>
       </c>
       <c r="AB49" s="31">
-        <f>P49-Y49</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC49" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD49" s="31">
-        <f>P49-N49-O49</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="50" spans="1:31" s="12" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="50" spans="1:31" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A50" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B50" s="13">
+      <c r="B50" s="22">
         <v>1</v>
       </c>
-      <c r="C50" s="13">
-        <f t="shared" si="3"/>
+      <c r="C50" s="22">
+        <f t="shared" si="6"/>
         <v>607199.50936786854</v>
       </c>
-      <c r="D50" s="13">
+      <c r="D50" s="22">
         <v>521648.45740734658</v>
       </c>
-      <c r="E50" s="13">
+      <c r="E50" s="22">
         <v>85551.051960521916</v>
       </c>
-      <c r="F50" s="13">
-        <f t="shared" si="4"/>
+      <c r="F50" s="22">
+        <f t="shared" si="7"/>
         <v>1068496.4843472885</v>
       </c>
-      <c r="G50" s="13">
+      <c r="G50" s="22">
         <v>639708.7667551405</v>
       </c>
-      <c r="H50" s="13">
+      <c r="H50" s="22">
         <v>94033.686897506646</v>
       </c>
-      <c r="I50" s="13">
+      <c r="I50" s="22">
         <v>334754.03069464129</v>
       </c>
-      <c r="J50" s="13">
-        <f t="shared" si="5"/>
+      <c r="J50" s="22">
+        <f t="shared" si="10"/>
         <v>2136301.3151854496</v>
       </c>
-      <c r="K50" s="13">
+      <c r="K50" s="22">
         <v>645038.51215367275</v>
       </c>
-      <c r="L50" s="13">
+      <c r="L50" s="22">
         <v>1017115.053259789</v>
       </c>
-      <c r="M50" s="13">
+      <c r="M50" s="22">
         <v>474147.74977198779</v>
       </c>
-      <c r="N50" s="13">
+      <c r="N50" s="22">
         <v>3811997.3089006068</v>
       </c>
-      <c r="O50" s="13">
+      <c r="O50" s="22">
         <v>279486.19468176691</v>
       </c>
-      <c r="P50" s="13">
+      <c r="P50" s="22">
         <v>4091483.5035823737</v>
       </c>
-      <c r="Q50" s="13">
+      <c r="Q50" s="22">
         <v>2286467.5630832217</v>
       </c>
-      <c r="R50" s="13">
+      <c r="R50" s="22">
         <v>415960.83765736083</v>
       </c>
-      <c r="S50" s="13">
+      <c r="S50" s="22">
         <v>1414917.7524715541</v>
       </c>
-      <c r="T50" s="13">
+      <c r="T50" s="22">
         <v>45182.100602970771</v>
       </c>
-      <c r="U50" s="13">
+      <c r="U50" s="22">
         <v>27991.062974024862</v>
       </c>
-      <c r="V50" s="13">
+      <c r="V50" s="22">
         <v>873874.93237120111</v>
       </c>
-      <c r="W50" s="13">
+      <c r="W50" s="22">
         <v>1105210.185037178</v>
       </c>
-      <c r="X50" s="13">
+      <c r="X50" s="22">
         <v>132299.43945921818</v>
       </c>
-      <c r="Y50" s="13">
+      <c r="Y50" s="22">
         <v>4091483.5035823737</v>
       </c>
-      <c r="Z50" s="13" t="s">
+      <c r="Z50" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="AA50" s="13">
+      <c r="AA50" s="22">
         <v>1</v>
       </c>
-      <c r="AB50" s="31">
-        <f>P50-Y50</f>
+      <c r="AB50" s="34">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC50" s="31">
-        <f t="shared" si="6"/>
+      <c r="AC50" s="34">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD50" s="31">
-        <f>P50-N50-O50</f>
+      <c r="AD50" s="34">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AE50" s="13"/>
-    </row>
-    <row r="51" spans="1:31" x14ac:dyDescent="0.35">
+      <c r="AE50" s="22"/>
+    </row>
+    <row r="51" spans="1:31" s="30" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A51" s="30" t="s">
         <v>135</v>
       </c>
-      <c r="B51" s="13">
+      <c r="B51" s="22">
         <v>2</v>
       </c>
-      <c r="C51" s="13">
-        <f t="shared" si="3"/>
+      <c r="C51" s="22">
+        <f t="shared" si="6"/>
         <v>509922.75262524036</v>
       </c>
-      <c r="D51" s="13">
+      <c r="D51" s="22">
         <v>440988.76929819351</v>
       </c>
-      <c r="E51" s="13">
+      <c r="E51" s="22">
         <v>68933.983327046823</v>
       </c>
-      <c r="F51" s="13">
-        <f t="shared" si="4"/>
+      <c r="F51" s="22">
+        <f t="shared" si="7"/>
         <v>1104935.8028121369</v>
       </c>
-      <c r="G51" s="13">
+      <c r="G51" s="22">
         <v>687182.77001122152</v>
       </c>
-      <c r="H51" s="13">
+      <c r="H51" s="22">
         <v>97686.029606063472</v>
       </c>
-      <c r="I51" s="13">
+      <c r="I51" s="22">
         <v>320067.00319485192</v>
       </c>
-      <c r="J51" s="13">
-        <f t="shared" si="5"/>
+      <c r="J51" s="22">
+        <f t="shared" si="10"/>
         <v>2227614.757630887</v>
       </c>
-      <c r="K51" s="13">
+      <c r="K51" s="22">
         <v>707674.84797380981</v>
       </c>
-      <c r="L51" s="13">
+      <c r="L51" s="22">
         <v>1011847.3003571649</v>
       </c>
-      <c r="M51" s="13">
+      <c r="M51" s="22">
         <v>508092.60929991212</v>
       </c>
-      <c r="N51" s="13">
+      <c r="N51" s="22">
         <v>3842473.3130682642</v>
       </c>
-      <c r="O51" s="13">
+      <c r="O51" s="22">
         <v>343306.12314272515</v>
       </c>
-      <c r="P51" s="13">
+      <c r="P51" s="22">
         <v>4185779.4362109895</v>
       </c>
-      <c r="Q51" s="13">
+      <c r="Q51" s="22">
         <v>2342610.3243549457</v>
       </c>
-      <c r="R51" s="13">
+      <c r="R51" s="22">
         <v>383709.08992555569</v>
       </c>
-      <c r="S51" s="13">
+      <c r="S51" s="22">
         <v>1435078.8054030915</v>
       </c>
-      <c r="T51" s="13">
+      <c r="T51" s="22">
         <v>48535.150150848924</v>
       </c>
-      <c r="U51" s="13">
+      <c r="U51" s="22">
         <v>108733.18162371332</v>
       </c>
-      <c r="V51" s="13">
+      <c r="V51" s="22">
         <v>996098.17064637633</v>
       </c>
-      <c r="W51" s="13">
+      <c r="W51" s="22">
         <v>1147928.0569367262</v>
       </c>
-      <c r="X51" s="13">
+      <c r="X51" s="22">
         <v>18942.771043184912</v>
       </c>
-      <c r="Y51" s="13">
+      <c r="Y51" s="22">
         <v>4185779.43621099</v>
       </c>
-      <c r="Z51" s="13" t="s">
+      <c r="Z51" s="22" t="s">
         <v>135</v>
       </c>
-      <c r="AA51" s="13">
+      <c r="AA51" s="22">
         <v>2</v>
       </c>
-      <c r="AB51" s="31">
-        <f>P51-Y51</f>
+      <c r="AB51" s="34">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC51" s="31">
-        <f t="shared" si="6"/>
+      <c r="AC51" s="34">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD51" s="31">
-        <f>P51-N51-O51</f>
+      <c r="AD51" s="34">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
+      <c r="AE51" s="22"/>
     </row>
     <row r="52" spans="1:31" x14ac:dyDescent="0.35">
       <c r="A52" s="30" t="s">
@@ -20456,7 +20459,7 @@
         <v>82645.205360628446</v>
       </c>
       <c r="F52" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1104725.5926862303</v>
       </c>
       <c r="G52" s="13">
@@ -20469,7 +20472,7 @@
         <v>361170.36766488163</v>
       </c>
       <c r="J52" s="13">
-        <f t="shared" si="5"/>
+        <f t="shared" si="10"/>
         <v>2096995.6475848635</v>
       </c>
       <c r="K52" s="13">
@@ -20524,15 +20527,15 @@
         <v>3</v>
       </c>
       <c r="AB52" s="31">
-        <f>P52-Y52</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC52" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD52" s="31">
-        <f>P52-N52-O52</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
@@ -20544,7 +20547,7 @@
         <v>4</v>
       </c>
       <c r="C53" s="13">
-        <f t="shared" si="3"/>
+        <f t="shared" si="6"/>
         <v>731379.25891265948</v>
       </c>
       <c r="D53" s="13">
@@ -20554,7 +20557,7 @@
         <v>100493.15544160279</v>
       </c>
       <c r="F53" s="13">
-        <f t="shared" si="4"/>
+        <f t="shared" si="7"/>
         <v>1283777.7292731942</v>
       </c>
       <c r="G53" s="13">
@@ -20622,124 +20625,210 @@
         <v>4</v>
       </c>
       <c r="AB53" s="31">
-        <f>P53-Y53</f>
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
       <c r="AC53" s="31">
-        <f t="shared" si="6"/>
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
       <c r="AD53" s="31">
-        <f>P53-N53-O53</f>
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
     </row>
-    <row r="54" spans="1:31" s="15" customFormat="1" x14ac:dyDescent="0.35">
+    <row r="54" spans="1:31" s="22" customFormat="1" x14ac:dyDescent="0.35">
       <c r="A54" s="30" t="s">
         <v>251</v>
       </c>
-      <c r="B54" s="13">
+      <c r="B54" s="22">
         <v>1</v>
       </c>
-      <c r="C54" s="13">
-        <f t="shared" si="3"/>
+      <c r="C54" s="22">
+        <f t="shared" si="6"/>
         <v>623783.6496154326</v>
       </c>
-      <c r="D54" s="13">
+      <c r="D54" s="22">
         <v>532092.16921362118</v>
       </c>
-      <c r="E54" s="13">
+      <c r="E54" s="22">
         <v>91691.480401811466</v>
       </c>
-      <c r="F54" s="13">
-        <f t="shared" si="4"/>
+      <c r="F54" s="22">
+        <f t="shared" si="7"/>
         <v>1158523.510813823</v>
       </c>
-      <c r="G54" s="13">
+      <c r="G54" s="22">
         <v>684792.14272417082</v>
       </c>
-      <c r="H54" s="13">
+      <c r="H54" s="22">
         <v>103804.51069326051</v>
       </c>
-      <c r="I54" s="13">
+      <c r="I54" s="22">
         <v>369926.8573963918</v>
       </c>
-      <c r="J54" s="13">
+      <c r="J54" s="22">
         <f>SUM(K54:M54)</f>
         <v>2290426.8797621289</v>
       </c>
-      <c r="K54" s="13">
+      <c r="K54" s="22">
         <v>681941.615617448</v>
       </c>
-      <c r="L54" s="13">
+      <c r="L54" s="22">
         <v>1089218.5938086153</v>
       </c>
-      <c r="M54" s="13">
+      <c r="M54" s="22">
         <v>519266.67033606535</v>
       </c>
-      <c r="N54" s="13">
+      <c r="N54" s="22">
         <v>4072734.0401913845</v>
       </c>
-      <c r="O54" s="13">
+      <c r="O54" s="22">
         <v>290997.84781663219</v>
       </c>
-      <c r="P54" s="13">
+      <c r="P54" s="22">
         <v>4363731.8880080171</v>
       </c>
-      <c r="Q54" s="13">
+      <c r="Q54" s="22">
         <v>2456777.2242074893</v>
       </c>
-      <c r="R54" s="13">
+      <c r="R54" s="22">
         <v>414944.76174693316</v>
       </c>
-      <c r="S54" s="13">
+      <c r="S54" s="22">
         <v>1520624.9806250322</v>
       </c>
-      <c r="T54" s="13">
+      <c r="T54" s="22">
         <v>47711.662507340596</v>
       </c>
-      <c r="U54" s="13">
+      <c r="U54" s="22">
         <v>24795.645138385869</v>
       </c>
-      <c r="V54" s="13">
+      <c r="V54" s="22">
         <v>949853.94812752737</v>
       </c>
-      <c r="W54" s="13">
+      <c r="W54" s="22">
         <v>1153942.9432330821</v>
       </c>
-      <c r="X54" s="13">
+      <c r="X54" s="22">
         <v>102966.60888838954</v>
       </c>
-      <c r="Y54" s="13">
+      <c r="Y54" s="22">
         <v>4363731.8880080162</v>
       </c>
-      <c r="Z54" s="13" t="s">
+      <c r="Z54" s="22" t="s">
         <v>251</v>
       </c>
-      <c r="AA54" s="13">
+      <c r="AA54" s="22">
         <v>1</v>
       </c>
-      <c r="AB54" s="31">
-        <f>P54-Y54</f>
+      <c r="AB54" s="34">
+        <f t="shared" si="8"/>
         <v>0</v>
       </c>
-      <c r="AC54" s="31">
-        <f t="shared" si="6"/>
+      <c r="AC54" s="34">
+        <f t="shared" si="11"/>
         <v>0</v>
       </c>
-      <c r="AD54" s="31">
-        <f>P54-N54-O54</f>
+      <c r="AD54" s="34">
+        <f t="shared" si="9"/>
         <v>0</v>
       </c>
-      <c r="AE54" s="13"/>
     </row>
     <row r="55" spans="1:31" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A55" s="22"/>
-      <c r="AD55" s="31"/>
-    </row>
-    <row r="56" spans="1:31" s="13" customFormat="1" x14ac:dyDescent="0.35">
-      <c r="A56" s="22"/>
-      <c r="AD56" s="31"/>
+      <c r="A55" s="30" t="s">
+        <v>251</v>
+      </c>
+      <c r="B55" s="13">
+        <v>2</v>
+      </c>
+      <c r="C55" s="13">
+        <v>525139.8819808457</v>
+      </c>
+      <c r="D55" s="13">
+        <v>456279.00593435531</v>
+      </c>
+      <c r="E55" s="13">
+        <v>68860.876046490346</v>
+      </c>
+      <c r="F55" s="13">
+        <v>1147522.7965168161</v>
+      </c>
+      <c r="G55" s="13">
+        <v>701960.72559979884</v>
+      </c>
+      <c r="H55" s="13">
+        <v>100922.31053666775</v>
+      </c>
+      <c r="I55" s="13">
+        <v>344639.76038034953</v>
+      </c>
+      <c r="J55" s="13">
+        <v>2385034.7147982363</v>
+      </c>
+      <c r="K55" s="13">
+        <v>750198.14055081154</v>
+      </c>
+      <c r="L55" s="13">
+        <v>1080050.5763129438</v>
+      </c>
+      <c r="M55" s="13">
+        <v>554785.9979344809</v>
+      </c>
+      <c r="N55" s="13">
+        <v>4057697.3932958981</v>
+      </c>
+      <c r="O55" s="13">
+        <v>352625.50972499058</v>
+      </c>
+      <c r="P55" s="13">
+        <v>4410322.9030208886</v>
+      </c>
+      <c r="Q55" s="13">
+        <v>2482287.7330999663</v>
+      </c>
+      <c r="R55" s="13">
+        <v>400698.15099968429</v>
+      </c>
+      <c r="S55" s="13">
+        <v>1513037.5101496552</v>
+      </c>
+      <c r="T55" s="13">
+        <v>49153.519748699204</v>
+      </c>
+      <c r="U55" s="13">
+        <v>124365.97748058324</v>
+      </c>
+      <c r="V55" s="13">
+        <v>1024347.2051186926</v>
+      </c>
+      <c r="W55" s="13">
+        <v>1114742.5369505414</v>
+      </c>
+      <c r="X55" s="13">
+        <v>-68824.656625850359</v>
+      </c>
+      <c r="Y55" s="13">
+        <v>4410322.9030208886</v>
+      </c>
+      <c r="Z55" s="22" t="s">
+        <v>251</v>
+      </c>
+      <c r="AA55" s="13">
+        <v>2</v>
+      </c>
+      <c r="AB55" s="31">
+        <f t="shared" ref="AB55" si="12">P55-Y55</f>
+        <v>0</v>
+      </c>
+      <c r="AC55" s="31">
+        <f t="shared" ref="AC55" si="13">N55-(C55+F55+J55)</f>
+        <v>0</v>
+      </c>
+      <c r="AD55" s="31">
+        <f t="shared" ref="AD55" si="14">P55-N55-O55</f>
+        <v>0</v>
+      </c>
     </row>
   </sheetData>
   <phoneticPr fontId="4" type="noConversion"/>

</xml_diff>